<commit_message>
save de excel a DB
</commit_message>
<xml_diff>
--- a/archivos_excel/historical.xlsx
+++ b/archivos_excel/historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EdoAndres\Descargas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0285C6-3728-4842-9DCC-FE5D79338FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87340887-0F49-44A3-8D03-584D8436AD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
     <t>Nombre archivo</t>
   </si>
   <si>
@@ -127,14 +124,17 @@
     <t>2023-02-17 19:00</t>
   </si>
   <si>
-    <t>id user</t>
+    <t>id audio</t>
+  </si>
+  <si>
+    <t>idusuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +151,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,90 +518,90 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>28</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
       </c>
       <c r="F2">
         <v>234.3</v>
@@ -654,19 +660,19 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>196.5</v>
@@ -725,19 +731,19 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>187.9</v>
@@ -796,19 +802,19 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>231.7</v>
@@ -867,19 +873,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>247.4</v>
@@ -938,19 +944,19 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>243.9</v>
@@ -1009,19 +1015,19 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>34</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>224.1</v>
@@ -1082,6 +1088,7 @@
       <c r="I16" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>